<commit_message>
Misc changes: 1. update config, 2. removal of validation results
</commit_message>
<xml_diff>
--- a/benchmarks/Results/Smart_Runtime/SmartRuntimeResults.xlsx
+++ b/benchmarks/Results/Smart_Runtime/SmartRuntimeResults.xlsx
@@ -1,22 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10614"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DebashisGanguly/Dropbox/SmartRuntime/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/DebashisGanguly/Downloads/gpgpu-sim_UVMSmart/benchmarks/Results/Smart_Runtime/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D367A0-CDE6-844B-AA03-2E6246024134}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3D4058-3AF7-7B4A-85B0-DF86F5C6099F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" activeTab="1" xr2:uid="{35D8FB26-F602-694F-A1A8-1D08C3A05AD8}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{35D8FB26-F602-694F-A1A8-1D08C3A05AD8}"/>
   </bookViews>
   <sheets>
-    <sheet name="ValidationPerformanceNoOver" sheetId="4" r:id="rId1"/>
-    <sheet name="ValidationMemcpyNoOversub" sheetId="3" r:id="rId2"/>
-    <sheet name="OversubPerformance" sheetId="1" r:id="rId3"/>
-    <sheet name="OversubThrashing" sheetId="2" r:id="rId4"/>
+    <sheet name="OversubPerformance" sheetId="1" r:id="rId1"/>
+    <sheet name="OversubThrashing" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="26">
   <si>
     <t>Unified</t>
   </si>
@@ -114,12 +112,6 @@
   </si>
   <si>
     <t>Unified Memory (Baseline)</t>
-  </si>
-  <si>
-    <t>GeForceGTX1080Ti</t>
-  </si>
-  <si>
-    <t>UVMSmart</t>
   </si>
 </sst>
 </file>
@@ -222,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -232,13 +224,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -250,10 +235,10 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -273,1126 +258,6 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ValidationPerformanceNoOver!$D$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GeForceGTX1080Ti</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>ValidationPerformanceNoOver!$B$17:$C$29</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2DCONV</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>BackProp</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pathfinder</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>StreamTriad</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>FDTD-2D</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Hotspot</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>SRAD_V2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>BFS</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>NW</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>SSSP</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>ATAX</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>RA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>GeoMean</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Streaming</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Regular</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Mixed</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Random</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Overall</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ValidationPerformanceNoOver!$D$17:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-8874-8B40-89C3-046352E55044}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ValidationPerformanceNoOver!$E$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UVMSmart</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>ValidationPerformanceNoOver!$B$17:$C$29</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2DCONV</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>BackProp</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pathfinder</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>StreamTriad</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>FDTD-2D</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Hotspot</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>SRAD_V2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>BFS</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>NW</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>SSSP</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>ATAX</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>RA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>GeoMean</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Streaming</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Regular</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Mixed</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Random</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Overall</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ValidationPerformanceNoOver!$E$17:$E$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>0.89646062749878108</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.83950008084120731</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.85498547012518955</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.87911350788122078</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.85512868136697839</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>0.80400653582244941</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3873200938637913</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1.1950187434038211</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.93285244106098786</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.1093014825592336</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.2127852814101685</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.1804727988503145</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.96075268340410636</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-8874-8B40-89C3-046352E55044}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="960713455"/>
-        <c:axId val="960715087"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="960713455"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="960715087"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="960715087"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.4"/>
-          <c:min val="0.60000000000000009"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" sz="1800" b="1">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                  </a:rPr>
-                  <a:t>Normalized Kernel Execution Time</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="960713455"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="1"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ValidationMemcpyNoOversub!$D$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>GeForceGTX1080Ti</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="65000"/>
-                <a:lumOff val="35000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>ValidationMemcpyNoOversub!$B$17:$C$29</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2DCONV</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>BackProp</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pathfinder</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>StreamTriad</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>FDTD-2D</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Hotspot</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>SRAD_V2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>BFS</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>NW</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>SSSP</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>ATAX</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>RA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>GeoMean</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Streaming</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Regular</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Mixed</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Random</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Overall</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ValidationMemcpyNoOversub!$D$17:$D$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-9338-244C-9EFF-A729499470AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>ValidationMemcpyNoOversub!$E$16</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>UVMSmart</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="bg1">
-                <a:lumMod val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:multiLvlStrRef>
-              <c:f>ValidationMemcpyNoOversub!$B$17:$C$29</c:f>
-              <c:multiLvlStrCache>
-                <c:ptCount val="13"/>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>2DCONV</c:v>
-                  </c:pt>
-                  <c:pt idx="1">
-                    <c:v>BackProp</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Pathfinder</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>StreamTriad</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>FDTD-2D</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Hotspot</c:v>
-                  </c:pt>
-                  <c:pt idx="6">
-                    <c:v>SRAD_V2</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>BFS</c:v>
-                  </c:pt>
-                  <c:pt idx="8">
-                    <c:v>NW</c:v>
-                  </c:pt>
-                  <c:pt idx="9">
-                    <c:v>SSSP</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>ATAX</c:v>
-                  </c:pt>
-                  <c:pt idx="11">
-                    <c:v>RA</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>GeoMean</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Streaming</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Regular</c:v>
-                  </c:pt>
-                  <c:pt idx="7">
-                    <c:v>Mixed</c:v>
-                  </c:pt>
-                  <c:pt idx="10">
-                    <c:v>Random</c:v>
-                  </c:pt>
-                  <c:pt idx="12">
-                    <c:v>Overall</c:v>
-                  </c:pt>
-                </c:lvl>
-              </c:multiLvlStrCache>
-            </c:multiLvlStrRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>ValidationMemcpyNoOversub!$E$17:$E$29</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="13"/>
-                <c:pt idx="0">
-                  <c:v>1.1806778859105604</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.86020473402673292</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.87503593820019587</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.86443225806978152</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>0.96133471577164975</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>1.3643602349846422</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>1.3565309034034421</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>0.77971139815366286</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>0.95261650562752165</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>1.0925061758284627</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.85747196196008624</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.1161257225208987</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>0.96325534589578865</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-9338-244C-9EFF-A729499470AD}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="934745103"/>
-        <c:axId val="934393999"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="934745103"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1"/>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="934393999"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="934393999"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-          <c:max val="1.4"/>
-          <c:min val="0.60000000000000009"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1"/>
-                    </a:solidFill>
-                    <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Normalized Host-to-device</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> Unified Memory Copy Time</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1"/>
-                  </a:solidFill>
-                  <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="934745103"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="t"/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1800" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="Times" pitchFamily="2" charset="0"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:noFill/>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-US"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -2520,7 +1385,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3671,86 +2536,6 @@
 </cs:colorStyle>
 </file>
 
-<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
-<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
-  <a:schemeClr val="accent1"/>
-  <a:schemeClr val="accent2"/>
-  <a:schemeClr val="accent3"/>
-  <a:schemeClr val="accent4"/>
-  <a:schemeClr val="accent5"/>
-  <a:schemeClr val="accent6"/>
-  <cs:variation/>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-    <a:lumOff val="20000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="80000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="60000"/>
-    <a:lumOff val="40000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-    <a:lumOff val="30000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="70000"/>
-  </cs:variation>
-  <cs:variation>
-    <a:lumMod val="50000"/>
-    <a:lumOff val="50000"/>
-  </cs:variation>
-</cs:colorStyle>
-</file>
-
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -4757,1095 +3542,7 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
-<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>819150</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>412750</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{201BD4A6-3406-EA41-9335-0263AAC3F00F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>63500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>482600</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{89901E38-A5B3-C54A-BFE8-611047647F09}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -5886,7 +3583,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -6223,834 +3920,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{848BA135-7486-A741-A475-93F552C1E156}">
-  <dimension ref="B2:H30"/>
-  <sheetViews>
-    <sheetView topLeftCell="D13" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2051</v>
-      </c>
-      <c r="E3" s="2">
-        <v>1838.6407469999999</v>
-      </c>
-      <c r="H3" s="9"/>
-    </row>
-    <row r="4" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>8720.7999999999993</v>
-      </c>
-      <c r="E4" s="2">
-        <v>7321.1123049999997</v>
-      </c>
-      <c r="H4" s="9"/>
-    </row>
-    <row r="5" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2">
-        <v>10544</v>
-      </c>
-      <c r="E5" s="2">
-        <v>9014.9667969999991</v>
-      </c>
-      <c r="H5" s="9"/>
-    </row>
-    <row r="6" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2">
-        <v>3387.8</v>
-      </c>
-      <c r="E6" s="2">
-        <v>2978.2607419999999</v>
-      </c>
-      <c r="H6" s="9"/>
-    </row>
-    <row r="7" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5710.99</v>
-      </c>
-      <c r="E7" s="2">
-        <v>4883.6313479999999</v>
-      </c>
-      <c r="H7" s="9"/>
-    </row>
-    <row r="8" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
-        <v>4226.3999999999996</v>
-      </c>
-      <c r="E8" s="2">
-        <v>3398.0532229999999</v>
-      </c>
-      <c r="H8" s="9"/>
-    </row>
-    <row r="9" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
-        <v>3108.76</v>
-      </c>
-      <c r="E9" s="2">
-        <v>4312.8452150000003</v>
-      </c>
-      <c r="H9" s="9"/>
-    </row>
-    <row r="10" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2">
-        <v>3217.7719999999999</v>
-      </c>
-      <c r="E10" s="2">
-        <v>3845.2978520000001</v>
-      </c>
-      <c r="H10" s="9"/>
-    </row>
-    <row r="11" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2">
-        <v>2916.15</v>
-      </c>
-      <c r="E11" s="2">
-        <v>2720.3376459999999</v>
-      </c>
-      <c r="H11" s="9"/>
-    </row>
-    <row r="12" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2">
-        <v>7972.7</v>
-      </c>
-      <c r="E12" s="2">
-        <v>8844.1279300000006</v>
-      </c>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2">
-        <v>2261.29</v>
-      </c>
-      <c r="E13" s="2">
-        <v>2742.4592290000001</v>
-      </c>
-      <c r="H13" s="9"/>
-    </row>
-    <row r="14" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2">
-        <v>4418.6000000000004</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5216.0371089999999</v>
-      </c>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="16" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2">
-        <f t="shared" ref="D17:D28" si="0">D3/D3</f>
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <f t="shared" ref="E17:E28" si="1">E3/D3</f>
-        <v>0.89646062749878108</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" si="1"/>
-        <v>0.83950008084120731</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.85498547012518955</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-      <c r="C20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.87911350788122078</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.85512868136697839</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="1"/>
-        <v>0.80400653582244941</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3873200938637913</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" si="1"/>
-        <v>1.1950187434038211</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.93285244106098786</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="1"/>
-        <v>1.1093014825592336</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="1"/>
-        <v>1.2127852814101685</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="1"/>
-        <v>1.1804727988503145</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B29" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="6">
-        <f>GEOMEAN(D17:D28)</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="6">
-        <f>GEOMEAN(E17,E18,E20,E21,E25,E27,E28)</f>
-        <v>0.96075268340410636</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B30" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B23"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B3B0231-79AD-3A4A-8A63-C7CE6FB5F8BA}">
-  <dimension ref="B2:H29"/>
-  <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D14" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H2" s="3"/>
-    </row>
-    <row r="3" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>593.91999999999996</v>
-      </c>
-      <c r="E3" s="2">
-        <v>701.22820999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B4" s="12"/>
-      <c r="C4" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="2">
-        <v>2743.5839999999998</v>
-      </c>
-      <c r="E4" s="2">
-        <v>2360.0439449999999</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
-      <c r="C5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="2">
-        <v>3856.0639999999999</v>
-      </c>
-      <c r="E5" s="2">
-        <v>3374.1945799999999</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="13"/>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="2">
-        <v>1225.3119999999999</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1059.1992190000001</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B7" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="2">
-        <v>1653.6</v>
-      </c>
-      <c r="E7" s="2">
-        <v>1589.663086</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="12"/>
-      <c r="C8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
-        <v>770.94399999999996</v>
-      </c>
-      <c r="E8" s="2">
-        <v>1051.845337</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B9" s="13"/>
-      <c r="C9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="2">
-        <v>1030.0160000000001</v>
-      </c>
-      <c r="E9" s="2">
-        <v>1397.2485349999999</v>
-      </c>
-    </row>
-    <row r="10" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D10" s="2">
-        <v>1182.0160000000001</v>
-      </c>
-      <c r="E10" s="2">
-        <v>921.631348</v>
-      </c>
-    </row>
-    <row r="11" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B11" s="12"/>
-      <c r="C11" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D11" s="2">
-        <v>753.44</v>
-      </c>
-      <c r="E11" s="2">
-        <v>717.73937999999998</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B12" s="13"/>
-      <c r="C12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2">
-        <v>2337.8240000000001</v>
-      </c>
-      <c r="E12" s="2">
-        <v>2554.0871579999998</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B13" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="2">
-        <v>683.072</v>
-      </c>
-      <c r="E13" s="2">
-        <v>585.71508800000004</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B14" s="13"/>
-      <c r="C14" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2">
-        <v>1029.7280000000001</v>
-      </c>
-      <c r="E14" s="2">
-        <v>1149.305908</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" ht="24" x14ac:dyDescent="0.3">
-      <c r="B16" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B17" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D17" s="2">
-        <f>D3/D3</f>
-        <v>1</v>
-      </c>
-      <c r="E17" s="2">
-        <f>E3/D3</f>
-        <v>1.1806778859105604</v>
-      </c>
-    </row>
-    <row r="18" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B18" s="12"/>
-      <c r="C18" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="2">
-        <f t="shared" ref="D18:D28" si="0">D4/D4</f>
-        <v>1</v>
-      </c>
-      <c r="E18" s="2">
-        <f t="shared" ref="E18:E28" si="1">E4/D4</f>
-        <v>0.86020473402673292</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B19" s="12"/>
-      <c r="C19" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D19" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E19" s="2">
-        <f t="shared" si="1"/>
-        <v>0.87503593820019587</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B20" s="13"/>
-      <c r="C20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D20" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E20" s="2">
-        <f t="shared" si="1"/>
-        <v>0.86443225806978152</v>
-      </c>
-    </row>
-    <row r="21" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B21" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="D21" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E21" s="2">
-        <f t="shared" si="1"/>
-        <v>0.96133471577164975</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B22" s="12"/>
-      <c r="C22" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E22" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3643602349846422</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B23" s="13"/>
-      <c r="C23" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D23" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E23" s="2">
-        <f t="shared" si="1"/>
-        <v>1.3565309034034421</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E24" s="2">
-        <f t="shared" si="1"/>
-        <v>0.77971139815366286</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B25" s="12"/>
-      <c r="C25" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D25" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E25" s="2">
-        <f t="shared" si="1"/>
-        <v>0.95261650562752165</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B26" s="13"/>
-      <c r="C26" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E26" s="2">
-        <f t="shared" si="1"/>
-        <v>1.0925061758284627</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B27" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D27" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E27" s="2">
-        <f t="shared" si="1"/>
-        <v>0.85747196196008624</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
-      <c r="C28" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D28" s="2">
-        <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="E28" s="2">
-        <f t="shared" si="1"/>
-        <v>1.1161257225208987</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" ht="24" x14ac:dyDescent="0.3">
-      <c r="B29" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="C29" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D29" s="6">
-        <f>GEOMEAN(D17:D28)</f>
-        <v>1</v>
-      </c>
-      <c r="E29" s="6">
-        <f>GEOMEAN(E17,E18,E20,E21,E25,E27,E28)</f>
-        <v>0.96325534589578865</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="B17:B20"/>
-    <mergeCell ref="B21:B23"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="B27:B28"/>
-    <mergeCell ref="B3:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B14"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3373ED2A-EF49-0740-ADC1-A4851EC9A0A2}">
   <dimension ref="B2:G35"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="68" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="68" workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -7067,14 +3940,14 @@
     <row r="2" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>125</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12">
         <v>150</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -7097,7 +3970,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -7117,7 +3990,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
@@ -7135,7 +4008,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="12"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
@@ -7153,7 +4026,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
@@ -7171,7 +4044,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -7191,7 +4064,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
@@ -7209,7 +4082,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
@@ -7227,7 +4100,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -7247,7 +4120,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -7265,7 +4138,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -7283,7 +4156,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -7303,7 +4176,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
@@ -7323,14 +4196,14 @@
     <row r="17" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
@@ -7353,7 +4226,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="11" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -7377,7 +4250,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B20" s="15"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
@@ -7399,7 +4272,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B21" s="15"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
@@ -7421,7 +4294,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B22" s="15"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
@@ -7443,7 +4316,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B23" s="15"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="5" t="s">
         <v>20</v>
       </c>
@@ -7465,7 +4338,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="11" t="s">
         <v>17</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -7489,7 +4362,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B25" s="15"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="3" t="s">
         <v>7</v>
       </c>
@@ -7511,7 +4384,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B26" s="15"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="3" t="s">
         <v>10</v>
       </c>
@@ -7533,7 +4406,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B27" s="15"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="5" t="s">
         <v>20</v>
       </c>
@@ -7555,7 +4428,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="3" t="s">
@@ -7579,7 +4452,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B29" s="15"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="3" t="s">
         <v>8</v>
       </c>
@@ -7601,7 +4474,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B30" s="15"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="3" t="s">
         <v>11</v>
       </c>
@@ -7623,7 +4496,7 @@
       </c>
     </row>
     <row r="31" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B31" s="15"/>
+      <c r="B31" s="11"/>
       <c r="C31" s="4" t="s">
         <v>20</v>
       </c>
@@ -7645,7 +4518,7 @@
       </c>
     </row>
     <row r="32" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C32" s="3" t="s">
@@ -7669,7 +4542,7 @@
       </c>
     </row>
     <row r="33" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B33" s="15"/>
+      <c r="B33" s="11"/>
       <c r="C33" s="3" t="s">
         <v>13</v>
       </c>
@@ -7691,7 +4564,7 @@
       </c>
     </row>
     <row r="34" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B34" s="15"/>
+      <c r="B34" s="11"/>
       <c r="C34" s="4" t="s">
         <v>20</v>
       </c>
@@ -7738,29 +4611,29 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="B4:B7"/>
+    <mergeCell ref="B8:B10"/>
+    <mergeCell ref="D17:E17"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="F17:G17"/>
     <mergeCell ref="B19:B23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B28:B31"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B4:B7"/>
-    <mergeCell ref="B8:B10"/>
-    <mergeCell ref="D17:E17"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="F17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8002C348-4B46-8A47-B49B-9805BCDB4D29}">
   <dimension ref="B2:G30"/>
   <sheetViews>
-    <sheetView topLeftCell="G9" zoomScale="75" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="75" workbookViewId="0">
       <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
@@ -7777,14 +4650,14 @@
     <row r="2" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="14">
+      <c r="D2" s="12">
         <v>125</v>
       </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14">
+      <c r="E2" s="12"/>
+      <c r="F2" s="12">
         <v>150</v>
       </c>
-      <c r="G2" s="14"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -7807,7 +4680,7 @@
       </c>
     </row>
     <row r="4" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -7827,7 +4700,7 @@
       </c>
     </row>
     <row r="5" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B5" s="12"/>
+      <c r="B5" s="9"/>
       <c r="C5" s="3" t="s">
         <v>5</v>
       </c>
@@ -7845,7 +4718,7 @@
       </c>
     </row>
     <row r="6" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B6" s="12"/>
+      <c r="B6" s="9"/>
       <c r="C6" s="3" t="s">
         <v>9</v>
       </c>
@@ -7863,7 +4736,7 @@
       </c>
     </row>
     <row r="7" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B7" s="13"/>
+      <c r="B7" s="10"/>
       <c r="C7" s="3" t="s">
         <v>12</v>
       </c>
@@ -7881,7 +4754,7 @@
       </c>
     </row>
     <row r="8" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
@@ -7901,7 +4774,7 @@
       </c>
     </row>
     <row r="9" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B9" s="12"/>
+      <c r="B9" s="9"/>
       <c r="C9" s="3" t="s">
         <v>7</v>
       </c>
@@ -7919,7 +4792,7 @@
       </c>
     </row>
     <row r="10" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B10" s="13"/>
+      <c r="B10" s="10"/>
       <c r="C10" s="3" t="s">
         <v>10</v>
       </c>
@@ -7937,7 +4810,7 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -7957,7 +4830,7 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B12" s="12"/>
+      <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
@@ -7975,7 +4848,7 @@
       </c>
     </row>
     <row r="13" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B13" s="13"/>
+      <c r="B13" s="10"/>
       <c r="C13" s="3" t="s">
         <v>11</v>
       </c>
@@ -7993,7 +4866,7 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B14" s="11" t="s">
+      <c r="B14" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
@@ -8013,7 +4886,7 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B15" s="13"/>
+      <c r="B15" s="10"/>
       <c r="C15" s="3" t="s">
         <v>13</v>
       </c>
@@ -8033,14 +4906,14 @@
     <row r="17" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B17" s="1"/>
       <c r="C17" s="2"/>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14" t="s">
+      <c r="E17" s="12"/>
+      <c r="F17" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="G17" s="14"/>
+      <c r="G17" s="12"/>
     </row>
     <row r="18" spans="2:7" ht="24" x14ac:dyDescent="0.3">
       <c r="B18" s="3" t="s">
@@ -8063,7 +4936,7 @@
       </c>
     </row>
     <row r="19" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B19" s="11" t="s">
+      <c r="B19" s="8" t="s">
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -8087,7 +4960,7 @@
       </c>
     </row>
     <row r="20" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B20" s="12"/>
+      <c r="B20" s="9"/>
       <c r="C20" s="3" t="s">
         <v>5</v>
       </c>
@@ -8109,7 +4982,7 @@
       </c>
     </row>
     <row r="21" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B21" s="12"/>
+      <c r="B21" s="9"/>
       <c r="C21" s="3" t="s">
         <v>9</v>
       </c>
@@ -8131,7 +5004,7 @@
       </c>
     </row>
     <row r="22" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B22" s="13"/>
+      <c r="B22" s="10"/>
       <c r="C22" s="3" t="s">
         <v>12</v>
       </c>
@@ -8153,7 +5026,7 @@
       </c>
     </row>
     <row r="23" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B23" s="11" t="s">
+      <c r="B23" s="8" t="s">
         <v>17</v>
       </c>
       <c r="C23" s="3" t="s">
@@ -8177,7 +5050,7 @@
       </c>
     </row>
     <row r="24" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B24" s="12"/>
+      <c r="B24" s="9"/>
       <c r="C24" s="3" t="s">
         <v>7</v>
       </c>
@@ -8199,7 +5072,7 @@
       </c>
     </row>
     <row r="25" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B25" s="13"/>
+      <c r="B25" s="10"/>
       <c r="C25" s="3" t="s">
         <v>10</v>
       </c>
@@ -8221,7 +5094,7 @@
       </c>
     </row>
     <row r="26" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B26" s="11" t="s">
+      <c r="B26" s="8" t="s">
         <v>18</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -8245,7 +5118,7 @@
       </c>
     </row>
     <row r="27" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B27" s="12"/>
+      <c r="B27" s="9"/>
       <c r="C27" s="3" t="s">
         <v>8</v>
       </c>
@@ -8267,7 +5140,7 @@
       </c>
     </row>
     <row r="28" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B28" s="13"/>
+      <c r="B28" s="10"/>
       <c r="C28" s="3" t="s">
         <v>11</v>
       </c>
@@ -8289,7 +5162,7 @@
       </c>
     </row>
     <row r="29" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B29" s="11" t="s">
+      <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -8313,7 +5186,7 @@
       </c>
     </row>
     <row r="30" spans="2:7" ht="24" x14ac:dyDescent="0.3">
-      <c r="B30" s="13"/>
+      <c r="B30" s="10"/>
       <c r="C30" s="3" t="s">
         <v>13</v>
       </c>

</xml_diff>